<commit_message>
Fixing the issue related to GD spreadsheet not being automatically open in excel
- Fixing the issue related to GD spreadsheet not being automatically open in excel
- Updating the indexer lib spreadsheet data
</commit_message>
<xml_diff>
--- a/indexer_lib/data/Poupanca.xlsx
+++ b/indexer_lib/data/Poupanca.xlsx
@@ -482,7 +482,9 @@
       <c r="B2" s="3">
         <v>0.55000000000000004</v>
       </c>
-      <c r="C2" s="3"/>
+      <c r="C2" s="3">
+        <v>0.5</v>
+      </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>

</xml_diff>

<commit_message>
Updating the indexer lib data folder
Updating the indexer lib data folder with data from March/2022
</commit_message>
<xml_diff>
--- a/indexer_lib/data/Poupanca.xlsx
+++ b/indexer_lib/data/Poupanca.xlsx
@@ -485,7 +485,9 @@
       <c r="C2" s="3">
         <v>0.5</v>
       </c>
-      <c r="D2" s="3"/>
+      <c r="D2" s="3">
+        <v>0.61</v>
+      </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>

</xml_diff>

<commit_message>
Workaround to show the Current Total Invested Value
- Workaround to show the Current Total Invested Value
- Updating the data folder in 'indexer_lib'
</commit_message>
<xml_diff>
--- a/indexer_lib/data/Poupanca.xlsx
+++ b/indexer_lib/data/Poupanca.xlsx
@@ -491,7 +491,9 @@
       <c r="E2" s="3">
         <v>0.66</v>
       </c>
-      <c r="F2" s="3"/>
+      <c r="F2" s="3">
+        <v>0.61</v>
+      </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>

</xml_diff>

<commit_message>
Updating 'indexer_lib\data' folder with August\2022 values
</commit_message>
<xml_diff>
--- a/indexer_lib/data/Poupanca.xlsx
+++ b/indexer_lib/data/Poupanca.xlsx
@@ -500,7 +500,9 @@
       <c r="H2" s="3">
         <v>0.71</v>
       </c>
-      <c r="I2" s="3"/>
+      <c r="I2" s="3">
+        <v>0.73719999999999997</v>
+      </c>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>

</xml_diff>

<commit_message>
Updating indexer lib with dec/2022 data
</commit_message>
<xml_diff>
--- a/indexer_lib/data/Poupanca.xlsx
+++ b/indexer_lib/data/Poupanca.xlsx
@@ -512,7 +512,9 @@
       <c r="K2" s="3">
         <v>0.65010000000000001</v>
       </c>
-      <c r="L2" s="3"/>
+      <c r="L2" s="3">
+        <v>0.65149999999999997</v>
+      </c>
       <c r="M2" s="3"/>
       <c r="O2" t="s">
         <v>16</v>

</xml_diff>